<commit_message>
Changes for ISsue fixes
Changes for ISsue fixes
</commit_message>
<xml_diff>
--- a/01_Requirements/Firm BS Horizontal Format.xlsx
+++ b/01_Requirements/Firm BS Horizontal Format.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IIT's\Accounting Reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\IIT\01_Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712E334E-1E0C-4D0D-AC8B-06A2E92726A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F43BDC46-746D-4618-983B-BD2673360F1B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
   </bookViews>
   <sheets>
     <sheet name="Balance Sheet- Firm AOP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -267,10 +266,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -559,7 +558,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -596,7 +595,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -608,13 +607,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -638,7 +637,7 @@
     <xf numFmtId="0" fontId="2" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -647,7 +646,7 @@
     <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,20 +664,26 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="12" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="11" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="13" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -697,12 +702,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1018,11 +1017,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2C101E1-A611-42A1-9793-7503C5B1790E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:O111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" zoomScale="89" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1041,38 +1040,38 @@
   <sheetData>
     <row r="1" spans="2:15" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="43"/>
-      <c r="J2" s="40" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="45"/>
+      <c r="J2" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
     </row>
     <row r="3" spans="2:15" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="44" t="s">
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="45"/>
-      <c r="J3" s="40" t="s">
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="47"/>
+      <c r="J3" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L3" s="40"/>
-      <c r="M3" s="40"/>
-      <c r="N3" s="40"/>
-      <c r="O3" s="40" t="s">
+      <c r="L3" s="42"/>
+      <c r="M3" s="42"/>
+      <c r="N3" s="42"/>
+      <c r="O3" s="42" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1089,7 +1088,7 @@
       <c r="E4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J4" s="40"/>
+      <c r="J4" s="42"/>
       <c r="K4" s="4" t="s">
         <v>7</v>
       </c>
@@ -1102,7 +1101,7 @@
       <c r="N4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="40"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -1431,14 +1430,14 @@
       <c r="E17" s="27">
         <v>40</v>
       </c>
-      <c r="J17" s="40" t="s">
+      <c r="J17" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K17" s="40"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="40"/>
-      <c r="N17" s="40"/>
-      <c r="O17" s="40"/>
+      <c r="K17" s="42"/>
+      <c r="L17" s="42"/>
+      <c r="M17" s="42"/>
+      <c r="N17" s="42"/>
+      <c r="O17" s="42"/>
     </row>
     <row r="18" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="13" t="s">
@@ -1453,16 +1452,16 @@
       <c r="E18" s="27">
         <v>150</v>
       </c>
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K18" s="40" t="s">
+      <c r="K18" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L18" s="40"/>
-      <c r="M18" s="40"/>
-      <c r="N18" s="40"/>
-      <c r="O18" s="40" t="s">
+      <c r="L18" s="42"/>
+      <c r="M18" s="42"/>
+      <c r="N18" s="42"/>
+      <c r="O18" s="42" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1475,7 +1474,7 @@
       <c r="E19" s="27">
         <v>100</v>
       </c>
-      <c r="J19" s="40"/>
+      <c r="J19" s="42"/>
       <c r="K19" s="4" t="s">
         <v>7</v>
       </c>
@@ -1488,7 +1487,7 @@
       <c r="N19" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O19" s="40"/>
+      <c r="O19" s="42"/>
     </row>
     <row r="20" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="13"/>
@@ -1668,40 +1667,40 @@
         <f>E25-C25</f>
         <v>0</v>
       </c>
-      <c r="J26" s="46" t="s">
+      <c r="J26" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="K26" s="46"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46"/>
-      <c r="N26" s="46"/>
-      <c r="O26" s="46"/>
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
     </row>
     <row r="27" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="J28" s="40" t="s">
+      <c r="J28" s="42" t="s">
         <v>40</v>
       </c>
-      <c r="K28" s="40"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="40"/>
-      <c r="N28" s="40"/>
-      <c r="O28" s="40"/>
+      <c r="K28" s="42"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="42"/>
+      <c r="N28" s="42"/>
+      <c r="O28" s="42"/>
     </row>
     <row r="29" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="40" t="s">
+      <c r="J29" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K29" s="40" t="s">
+      <c r="K29" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L29" s="40"/>
-      <c r="M29" s="40"/>
-      <c r="N29" s="40"/>
-      <c r="O29" s="40" t="s">
+      <c r="L29" s="42"/>
+      <c r="M29" s="42"/>
+      <c r="N29" s="42"/>
+      <c r="O29" s="42" t="s">
         <v>5</v>
       </c>
     </row>
@@ -1709,7 +1708,7 @@
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J30" s="40"/>
+      <c r="J30" s="42"/>
       <c r="K30" s="4" t="s">
         <v>7</v>
       </c>
@@ -1722,7 +1721,7 @@
       <c r="N30" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O30" s="40"/>
+      <c r="O30" s="42"/>
     </row>
     <row r="31" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J31" s="7" t="s">
@@ -1756,12 +1755,12 @@
       <c r="O32" s="12"/>
     </row>
     <row r="33" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="40" t="s">
+      <c r="B33" s="42" t="s">
         <v>52</v>
       </c>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="40"/>
+      <c r="C33" s="42"/>
+      <c r="D33" s="42"/>
+      <c r="E33" s="42"/>
       <c r="J33" s="10" t="s">
         <v>46</v>
       </c>
@@ -1980,43 +1979,43 @@
         <f>SUM(E35:E39)</f>
         <v>705</v>
       </c>
-      <c r="J40" s="46" t="s">
+      <c r="J40" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="K40" s="46"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="46"/>
-      <c r="N40" s="46"/>
-      <c r="O40" s="46"/>
+      <c r="K40" s="41"/>
+      <c r="L40" s="41"/>
+      <c r="M40" s="41"/>
+      <c r="N40" s="41"/>
+      <c r="O40" s="41"/>
     </row>
     <row r="41" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="42" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J42" s="40" t="s">
+      <c r="J42" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="K42" s="40"/>
-      <c r="L42" s="40"/>
-      <c r="M42" s="40"/>
-      <c r="N42" s="40"/>
-      <c r="O42" s="40"/>
+      <c r="K42" s="42"/>
+      <c r="L42" s="42"/>
+      <c r="M42" s="42"/>
+      <c r="N42" s="42"/>
+      <c r="O42" s="42"/>
     </row>
     <row r="43" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="40" t="s">
+      <c r="B43" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="40"/>
-      <c r="D43" s="40"/>
-      <c r="E43" s="40"/>
-      <c r="J43" s="40" t="s">
+      <c r="C43" s="42"/>
+      <c r="D43" s="42"/>
+      <c r="E43" s="42"/>
+      <c r="J43" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="K43" s="40" t="s">
+      <c r="K43" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="L43" s="40"/>
-      <c r="M43" s="40"/>
-      <c r="N43" s="40"/>
-      <c r="O43" s="40" t="s">
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2033,7 +2032,7 @@
       <c r="E44" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="J44" s="40"/>
+      <c r="J44" s="42"/>
       <c r="K44" s="4" t="s">
         <v>7</v>
       </c>
@@ -2046,7 +2045,7 @@
       <c r="N44" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="O44" s="40"/>
+      <c r="O44" s="42"/>
     </row>
     <row r="45" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="10" t="s">
@@ -2224,22 +2223,22 @@
       </c>
     </row>
     <row r="51" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J51" s="46" t="s">
+      <c r="J51" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="K51" s="46"/>
-      <c r="L51" s="46"/>
-      <c r="M51" s="46"/>
-      <c r="N51" s="46"/>
-      <c r="O51" s="46"/>
+      <c r="K51" s="41"/>
+      <c r="L51" s="41"/>
+      <c r="M51" s="41"/>
+      <c r="N51" s="41"/>
+      <c r="O51" s="41"/>
     </row>
     <row r="52" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="47" t="s">
+      <c r="B52" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="C52" s="47"/>
-      <c r="D52" s="47"/>
-      <c r="E52" s="47"/>
+      <c r="C52" s="40"/>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
     </row>
     <row r="53" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="54" spans="2:15" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2302,6 +2301,18 @@
     <row r="111" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="J28:O28"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="J2:O2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="K3:N3"/>
+    <mergeCell ref="O3:O4"/>
+    <mergeCell ref="J17:O17"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="K18:N18"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="J26:O26"/>
     <mergeCell ref="B52:E52"/>
     <mergeCell ref="J51:O51"/>
     <mergeCell ref="J29:J30"/>
@@ -2314,18 +2325,6 @@
     <mergeCell ref="J43:J44"/>
     <mergeCell ref="K43:N43"/>
     <mergeCell ref="O43:O44"/>
-    <mergeCell ref="J28:O28"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="J2:O2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="J3:J4"/>
-    <mergeCell ref="K3:N3"/>
-    <mergeCell ref="O3:O4"/>
-    <mergeCell ref="J17:O17"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="K18:N18"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="J26:O26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>